<commit_message>
Update including mobile positive and negative scenario
</commit_message>
<xml_diff>
--- a/ITP0001-NEEDUS Product Sales Project Scenarios.xlsx
+++ b/ITP0001-NEEDUS Product Sales Project Scenarios.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="203">
   <si>
     <t>Effort Reference</t>
   </si>
@@ -250,7 +250,7 @@
     <t>Click Language</t>
   </si>
   <si>
-    <t>SCN0004-MS-Product details page upper menus, account options and buying</t>
+    <t>SCN0004-MS-Landing page newsletter subscription - Negative Scenario</t>
   </si>
   <si>
     <t>TC0030</t>
@@ -259,216 +259,216 @@
     <t>Access the Product details link</t>
   </si>
   <si>
+    <t>Access the product details link, fill newsletter email field with "test@test", click subscribe, empty email field, click subscribe.</t>
+  </si>
+  <si>
+    <t>TC0031</t>
+  </si>
+  <si>
+    <t>Fill Newsletter email field incorrectly</t>
+  </si>
+  <si>
+    <t>TC0032</t>
+  </si>
+  <si>
+    <t>Click Subscribe</t>
+  </si>
+  <si>
+    <t>TC0033</t>
+  </si>
+  <si>
+    <t>Click Subscribe while email field is empty</t>
+  </si>
+  <si>
+    <t>SCN0005-MS-Product details page upper menus, account options and buying</t>
+  </si>
+  <si>
+    <t>TC0034</t>
+  </si>
+  <si>
     <t>Access the product details link, click serach bar, check if all categories match PDP, click login, click signup, click endorse, click cart, check if home options match PDP, check if about options match PDP, check if product options match PDP, check if pages options match PDP, check if contact options match PDP, click support.</t>
   </si>
   <si>
-    <t>TC0031</t>
+    <t>TC0035</t>
   </si>
   <si>
     <t>Click the search bar</t>
   </si>
   <si>
-    <t>TC0032</t>
+    <t>TC0036</t>
   </si>
   <si>
     <t>Query All Categories</t>
   </si>
   <si>
-    <t>TC0033</t>
+    <t>TC0037</t>
   </si>
   <si>
     <t>Click Login</t>
   </si>
   <si>
-    <t>TC0034</t>
+    <t>TC0038</t>
   </si>
   <si>
     <t>Click Signup</t>
   </si>
   <si>
-    <t>TC0035</t>
+    <t>TC0039</t>
   </si>
   <si>
     <t>Click Endorse</t>
   </si>
   <si>
-    <t>TC0036</t>
+    <t>TC0040</t>
   </si>
   <si>
     <t>Click Cart</t>
   </si>
   <si>
-    <t>TC0037</t>
+    <t>TC0041</t>
   </si>
   <si>
     <t>Query All Categories options</t>
   </si>
   <si>
-    <t>TC0038</t>
+    <t>TC0042</t>
   </si>
   <si>
     <t>Query Home options</t>
   </si>
   <si>
-    <t>TC0039</t>
+    <t>TC0043</t>
   </si>
   <si>
     <t>Query About options</t>
   </si>
   <si>
-    <t>TC0040</t>
+    <t>TC0044</t>
   </si>
   <si>
     <t>Query Product options</t>
   </si>
   <si>
-    <t>TC0041</t>
+    <t>TC0045</t>
   </si>
   <si>
     <t>Query Pages options</t>
   </si>
   <si>
-    <t>TC0042</t>
+    <t>TC0046</t>
   </si>
   <si>
     <t>Query Contact options</t>
   </si>
   <si>
-    <t>TC0043</t>
+    <t>TC0047</t>
   </si>
   <si>
     <t>Click Support</t>
   </si>
   <si>
-    <t>SCN0005-MS-Product details page body current procuct, suggestions and newsletter</t>
-  </si>
-  <si>
-    <t>TC0044</t>
-  </si>
-  <si>
-    <t>Access the product details link, check if categories path match, click on product image list, click product advanced options, click quantity options, click buy now, click add to cart, check if description tab match PDP, check if specification tab match PDP, check if reviews tab match PDP, check suggested products list, check if nesletter title and description fill newsletter email input, click subscribe, fill newsletter email input, click subscribe.</t>
-  </si>
-  <si>
-    <t>TC0045</t>
+    <t>SCN006-MS-Product details page body current product, suggestions and newsletter</t>
+  </si>
+  <si>
+    <t>TC0048</t>
+  </si>
+  <si>
+    <t>Access the product details link, check if categories path match, click on product image list, click product advanced options, click quantity options, click buy now, click add to cart, check if description tab match PDP, check if specification tab match PDP, check if reviews tab match PDP, check suggested products list, check if newsletter title and description match PDP, fill newsletter email input, click subscribe, fill newsletter email input, click subscribe.</t>
+  </si>
+  <si>
+    <t>TC0049</t>
   </si>
   <si>
     <t>Query Categories path</t>
   </si>
   <si>
-    <t>TC0046</t>
+    <t>TC0050</t>
   </si>
   <si>
     <t>Click on Product Image list</t>
   </si>
   <si>
-    <t>TC0047</t>
+    <t>TC0051</t>
   </si>
   <si>
     <t>Click Product Advanced options</t>
   </si>
   <si>
-    <t>TC0048</t>
+    <t>TC0052</t>
   </si>
   <si>
     <t>Click Quantity Options</t>
   </si>
   <si>
-    <t>TC0049</t>
+    <t>TC0053</t>
   </si>
   <si>
     <t>Click Buy Now</t>
   </si>
   <si>
-    <t>TC0050</t>
+    <t>TC0054</t>
   </si>
   <si>
     <t>Click Add to Cart</t>
   </si>
   <si>
-    <t>TC0051</t>
+    <t>TC0055</t>
   </si>
   <si>
     <t>Query Description tab</t>
   </si>
   <si>
-    <t>TC0052</t>
+    <t>TC0056</t>
   </si>
   <si>
     <t>Query Specification tab</t>
   </si>
   <si>
-    <t>TC0053</t>
+    <t>TC0057</t>
   </si>
   <si>
     <t>Query Reviews tab</t>
   </si>
   <si>
-    <t>TC0054</t>
+    <t>TC0058</t>
   </si>
   <si>
     <t>Query Suggested products list</t>
   </si>
   <si>
-    <t>TC0055</t>
-  </si>
-  <si>
-    <t>SCN0006-MS-Product details page footer links and social media</t>
-  </si>
-  <si>
-    <t>TC0056</t>
+    <t>TC0059</t>
+  </si>
+  <si>
+    <t>SCN007-MS-Product details page footer links and social media</t>
+  </si>
+  <si>
+    <t>TC0060</t>
   </si>
   <si>
     <t>Access the product details link, check if about us title and description match PDP, click social media options, click information options, click account options, click store options, check if contact information match PDP.</t>
   </si>
   <si>
-    <t>TC0057</t>
-  </si>
-  <si>
-    <t>TC0058</t>
+    <t>TC0061</t>
+  </si>
+  <si>
+    <t>TC0062</t>
   </si>
   <si>
     <t>Click Information options</t>
   </si>
   <si>
-    <t>TC0059</t>
+    <t>TC0063</t>
   </si>
   <si>
     <t>Click Account options</t>
   </si>
   <si>
-    <t>TC0060</t>
+    <t>TC0064</t>
   </si>
   <si>
     <t>Click Store options</t>
   </si>
   <si>
-    <t>SCN0007-MS-Landing page newsletter subscription - Negative Scenario</t>
-  </si>
-  <si>
-    <t>TC0061</t>
-  </si>
-  <si>
-    <t>Access the product details link, fill newsletter email field with "test@test", click subscribe, empty email field, click subscribe.</t>
-  </si>
-  <si>
-    <t>TC0062</t>
-  </si>
-  <si>
-    <t>Fill Newsletter email field incorrectly</t>
-  </si>
-  <si>
-    <t>TC0063</t>
-  </si>
-  <si>
-    <t>Click Subscribe</t>
-  </si>
-  <si>
-    <t>TC0064</t>
-  </si>
-  <si>
-    <t>Click Subscribe while email field is empty</t>
-  </si>
-  <si>
     <t>SCN0008-MS-Product details search bar, buy now and newsletter - Negative Scenario</t>
   </si>
   <si>
@@ -494,13 +494,139 @@
   </si>
   <si>
     <t>TC0070</t>
+  </si>
+  <si>
+    <t>SCN0009-MS-Product details page - Mobile</t>
+  </si>
+  <si>
+    <t>TC0071</t>
+  </si>
+  <si>
+    <t>Access the product details link, click the upper left corner menu, check if categories match PDP, check if home match PDP, check if about match PDP, check if product match PDP, check if match PDP, check if contact match PDP, click search bar, fill current product name and search, click account, click endorse, click cart, check if categories path match PDP, click on a image in product image list, click buy now, click add to cart, check if description tab match PDP, check if specification tab match PDP, check if reviews tab match PDP, check if suggested products list match PDP, fill newsletter email input, click on subscribe, click about us, click information, click account, click store, click contact us.</t>
+  </si>
+  <si>
+    <t>TC0072</t>
+  </si>
+  <si>
+    <t>Click Menu</t>
+  </si>
+  <si>
+    <t>TC0073</t>
+  </si>
+  <si>
+    <t>TC0074</t>
+  </si>
+  <si>
+    <t>TC0075</t>
+  </si>
+  <si>
+    <t>TC0076</t>
+  </si>
+  <si>
+    <t>TC0077</t>
+  </si>
+  <si>
+    <t>TC0078</t>
+  </si>
+  <si>
+    <t>TC0079</t>
+  </si>
+  <si>
+    <t>TC0080</t>
+  </si>
+  <si>
+    <t>Click Account icon</t>
+  </si>
+  <si>
+    <t>TC0081</t>
+  </si>
+  <si>
+    <t>TC0082</t>
+  </si>
+  <si>
+    <t>TC0083</t>
+  </si>
+  <si>
+    <t>TC0084</t>
+  </si>
+  <si>
+    <t>TC0085</t>
+  </si>
+  <si>
+    <t>TC0086</t>
+  </si>
+  <si>
+    <t>TC0087</t>
+  </si>
+  <si>
+    <t>TC0088</t>
+  </si>
+  <si>
+    <t>TC0089</t>
+  </si>
+  <si>
+    <t>TC0090</t>
+  </si>
+  <si>
+    <t>TC0091</t>
+  </si>
+  <si>
+    <t>TC0092</t>
+  </si>
+  <si>
+    <t>Click About us</t>
+  </si>
+  <si>
+    <t>TC0093</t>
+  </si>
+  <si>
+    <t>Click Information</t>
+  </si>
+  <si>
+    <t>TC0094</t>
+  </si>
+  <si>
+    <t>Click Account</t>
+  </si>
+  <si>
+    <t>TC0095</t>
+  </si>
+  <si>
+    <t>Click Store</t>
+  </si>
+  <si>
+    <t>TC0096</t>
+  </si>
+  <si>
+    <t>Click Contact us</t>
+  </si>
+  <si>
+    <t>SCN0010-MS-Product details search bar, buy now and newsletter - Negative Scenario Mobile</t>
+  </si>
+  <si>
+    <t>TC0097</t>
+  </si>
+  <si>
+    <t>TC0098</t>
+  </si>
+  <si>
+    <t>TC0099</t>
+  </si>
+  <si>
+    <t>TC0100</t>
+  </si>
+  <si>
+    <t>TC0101</t>
+  </si>
+  <si>
+    <t>TC0102</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -513,6 +639,10 @@
       <scheme val="minor"/>
     </font>
     <font/>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -654,7 +784,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -690,6 +820,18 @@
     <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -912,7 +1054,7 @@
     <col customWidth="1" min="3" max="3" width="14.75"/>
     <col customWidth="1" min="4" max="4" width="2.13"/>
     <col customWidth="1" min="5" max="5" width="2.75"/>
-    <col customWidth="1" min="6" max="6" width="62.75"/>
+    <col customWidth="1" min="6" max="6" width="68.0"/>
     <col customWidth="1" min="7" max="7" width="4.75"/>
     <col customWidth="1" min="8" max="8" width="9.13"/>
     <col customWidth="1" min="9" max="9" width="6.5"/>
@@ -1518,7 +1660,7 @@
       <c r="L42" s="16"/>
     </row>
     <row r="43">
-      <c r="F43" s="8" t="s">
+      <c r="F43" s="17" t="s">
         <v>79</v>
       </c>
       <c r="G43" s="3" t="s">
@@ -1573,7 +1715,7 @@
       <c r="L45" s="13"/>
     </row>
     <row r="46">
-      <c r="F46" s="11"/>
+      <c r="F46" s="14"/>
       <c r="G46" s="3" t="s">
         <v>7</v>
       </c>
@@ -1586,11 +1728,13 @@
       <c r="J46" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="K46" s="12"/>
-      <c r="L46" s="13"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="16"/>
     </row>
     <row r="47">
-      <c r="F47" s="11"/>
+      <c r="F47" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="G47" s="3" t="s">
         <v>7</v>
       </c>
@@ -1598,13 +1742,15 @@
         <v>7</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="K47" s="12"/>
-      <c r="L47" s="13"/>
+        <v>81</v>
+      </c>
+      <c r="K47" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="L47" s="10"/>
     </row>
     <row r="48">
       <c r="F48" s="11"/>
@@ -1615,10 +1761,10 @@
         <v>7</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K48" s="12"/>
       <c r="L48" s="13"/>
@@ -1632,10 +1778,10 @@
         <v>7</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K49" s="12"/>
       <c r="L49" s="13"/>
@@ -1649,10 +1795,10 @@
         <v>7</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K50" s="12"/>
       <c r="L50" s="13"/>
@@ -1666,10 +1812,10 @@
         <v>7</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K51" s="12"/>
       <c r="L51" s="13"/>
@@ -1683,10 +1829,10 @@
         <v>7</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K52" s="12"/>
       <c r="L52" s="13"/>
@@ -1700,10 +1846,10 @@
         <v>7</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K53" s="12"/>
       <c r="L53" s="13"/>
@@ -1717,10 +1863,10 @@
         <v>7</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K54" s="12"/>
       <c r="L54" s="13"/>
@@ -1734,16 +1880,16 @@
         <v>7</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K55" s="12"/>
       <c r="L55" s="13"/>
     </row>
     <row r="56">
-      <c r="F56" s="14"/>
+      <c r="F56" s="11"/>
       <c r="G56" s="3" t="s">
         <v>7</v>
       </c>
@@ -1751,18 +1897,16 @@
         <v>7</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="K56" s="15"/>
-      <c r="L56" s="16"/>
+        <v>109</v>
+      </c>
+      <c r="K56" s="12"/>
+      <c r="L56" s="13"/>
     </row>
     <row r="57">
-      <c r="F57" s="8" t="s">
-        <v>109</v>
-      </c>
+      <c r="F57" s="11"/>
       <c r="G57" s="3" t="s">
         <v>7</v>
       </c>
@@ -1773,12 +1917,10 @@
         <v>110</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K57" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="L57" s="10"/>
+      <c r="K57" s="12"/>
+      <c r="L57" s="13"/>
     </row>
     <row r="58">
       <c r="F58" s="11"/>
@@ -1815,7 +1957,7 @@
       <c r="L59" s="13"/>
     </row>
     <row r="60">
-      <c r="F60" s="11"/>
+      <c r="F60" s="14"/>
       <c r="G60" s="3" t="s">
         <v>7</v>
       </c>
@@ -1828,11 +1970,13 @@
       <c r="J60" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="K60" s="12"/>
-      <c r="L60" s="13"/>
+      <c r="K60" s="15"/>
+      <c r="L60" s="16"/>
     </row>
     <row r="61">
-      <c r="F61" s="11"/>
+      <c r="F61" s="8" t="s">
+        <v>118</v>
+      </c>
       <c r="G61" s="3" t="s">
         <v>7</v>
       </c>
@@ -1840,13 +1984,15 @@
         <v>7</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="K61" s="12"/>
-      <c r="L61" s="13"/>
+        <v>81</v>
+      </c>
+      <c r="K61" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="L61" s="10"/>
     </row>
     <row r="62">
       <c r="F62" s="11"/>
@@ -1857,10 +2003,10 @@
         <v>7</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K62" s="12"/>
       <c r="L62" s="13"/>
@@ -1874,10 +2020,10 @@
         <v>7</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K63" s="12"/>
       <c r="L63" s="13"/>
@@ -1891,10 +2037,10 @@
         <v>7</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K64" s="12"/>
       <c r="L64" s="13"/>
@@ -1908,10 +2054,10 @@
         <v>7</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K65" s="12"/>
       <c r="L65" s="13"/>
@@ -1925,10 +2071,10 @@
         <v>7</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K66" s="12"/>
       <c r="L66" s="13"/>
@@ -1942,16 +2088,16 @@
         <v>7</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K67" s="12"/>
       <c r="L67" s="13"/>
     </row>
     <row r="68">
-      <c r="F68" s="14"/>
+      <c r="F68" s="11"/>
       <c r="G68" s="3" t="s">
         <v>7</v>
       </c>
@@ -1959,18 +2105,16 @@
         <v>7</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K68" s="15"/>
-      <c r="L68" s="16"/>
+        <v>134</v>
+      </c>
+      <c r="K68" s="12"/>
+      <c r="L68" s="13"/>
     </row>
     <row r="69">
-      <c r="F69" s="8" t="s">
-        <v>133</v>
-      </c>
+      <c r="F69" s="11"/>
       <c r="G69" s="3" t="s">
         <v>7</v>
       </c>
@@ -1978,15 +2122,13 @@
         <v>7</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K69" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="L69" s="10"/>
+        <v>136</v>
+      </c>
+      <c r="K69" s="12"/>
+      <c r="L69" s="13"/>
     </row>
     <row r="70">
       <c r="F70" s="11"/>
@@ -1997,10 +2139,10 @@
         <v>7</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="K70" s="12"/>
       <c r="L70" s="13"/>
@@ -2014,16 +2156,16 @@
         <v>7</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="K71" s="12"/>
       <c r="L71" s="13"/>
     </row>
     <row r="72">
-      <c r="F72" s="11"/>
+      <c r="F72" s="14"/>
       <c r="G72" s="3" t="s">
         <v>7</v>
       </c>
@@ -2031,16 +2173,18 @@
         <v>7</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="K72" s="12"/>
-      <c r="L72" s="13"/>
+        <v>51</v>
+      </c>
+      <c r="K72" s="15"/>
+      <c r="L72" s="16"/>
     </row>
     <row r="73">
-      <c r="F73" s="14"/>
+      <c r="F73" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="G73" s="3" t="s">
         <v>7</v>
       </c>
@@ -2048,18 +2192,18 @@
         <v>7</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="K73" s="15"/>
-      <c r="L73" s="16"/>
+        <v>81</v>
+      </c>
+      <c r="K73" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="L73" s="10"/>
     </row>
     <row r="74">
-      <c r="F74" s="17" t="s">
-        <v>143</v>
-      </c>
+      <c r="F74" s="11"/>
       <c r="G74" s="3" t="s">
         <v>7</v>
       </c>
@@ -2067,15 +2211,13 @@
         <v>7</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K74" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="L74" s="10"/>
+        <v>72</v>
+      </c>
+      <c r="K74" s="12"/>
+      <c r="L74" s="13"/>
     </row>
     <row r="75">
       <c r="F75" s="11"/>
@@ -2150,7 +2292,7 @@
       <c r="L78" s="10"/>
     </row>
     <row r="79">
-      <c r="F79" s="11"/>
+      <c r="F79" s="17"/>
       <c r="G79" s="3" t="s">
         <v>7</v>
       </c>
@@ -2167,7 +2309,7 @@
       <c r="L79" s="13"/>
     </row>
     <row r="80">
-      <c r="F80" s="11"/>
+      <c r="F80" s="17"/>
       <c r="G80" s="3" t="s">
         <v>7</v>
       </c>
@@ -2178,13 +2320,13 @@
         <v>157</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="K80" s="12"/>
       <c r="L80" s="13"/>
     </row>
     <row r="81">
-      <c r="F81" s="11"/>
+      <c r="F81" s="17"/>
       <c r="G81" s="3" t="s">
         <v>7</v>
       </c>
@@ -2195,13 +2337,13 @@
         <v>158</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>147</v>
+        <v>84</v>
       </c>
       <c r="K81" s="12"/>
       <c r="L81" s="13"/>
     </row>
     <row r="82">
-      <c r="F82" s="11"/>
+      <c r="F82" s="17"/>
       <c r="G82" s="3" t="s">
         <v>7</v>
       </c>
@@ -2212,13 +2354,13 @@
         <v>159</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="K82" s="12"/>
       <c r="L82" s="13"/>
     </row>
     <row r="83">
-      <c r="F83" s="14"/>
+      <c r="F83" s="18"/>
       <c r="G83" s="3" t="s">
         <v>7</v>
       </c>
@@ -2229,32 +2371,587 @@
         <v>160</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>151</v>
+        <v>88</v>
       </c>
       <c r="K83" s="15"/>
       <c r="L83" s="16"/>
     </row>
+    <row r="84">
+      <c r="F84" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="J84" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K84" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="L84" s="10"/>
+    </row>
+    <row r="85">
+      <c r="F85" s="11"/>
+      <c r="G85" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J85" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="K85" s="12"/>
+      <c r="L85" s="13"/>
+    </row>
+    <row r="86">
+      <c r="F86" s="11"/>
+      <c r="G86" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K86" s="12"/>
+      <c r="L86" s="13"/>
+    </row>
+    <row r="87">
+      <c r="F87" s="11"/>
+      <c r="G87" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="J87" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K87" s="12"/>
+      <c r="L87" s="13"/>
+    </row>
+    <row r="88">
+      <c r="F88" s="11"/>
+      <c r="G88" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="K88" s="12"/>
+      <c r="L88" s="13"/>
+    </row>
+    <row r="89">
+      <c r="F89" s="11"/>
+      <c r="G89" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="J89" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="K89" s="12"/>
+      <c r="L89" s="13"/>
+    </row>
+    <row r="90">
+      <c r="F90" s="11"/>
+      <c r="G90" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K90" s="12"/>
+      <c r="L90" s="13"/>
+    </row>
+    <row r="91">
+      <c r="F91" s="11"/>
+      <c r="G91" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I91" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="J91" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="K91" s="12"/>
+      <c r="L91" s="13"/>
+    </row>
+    <row r="92">
+      <c r="F92" s="11"/>
+      <c r="G92" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J92" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="K92" s="12"/>
+      <c r="L92" s="13"/>
+    </row>
+    <row r="93">
+      <c r="F93" s="11"/>
+      <c r="G93" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I93" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="J93" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="K93" s="12"/>
+      <c r="L93" s="13"/>
+    </row>
+    <row r="94">
+      <c r="F94" s="11"/>
+      <c r="G94" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="J94" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="K94" s="12"/>
+      <c r="L94" s="13"/>
+    </row>
+    <row r="95">
+      <c r="F95" s="11"/>
+      <c r="G95" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I95" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="J95" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="K95" s="12"/>
+      <c r="L95" s="13"/>
+    </row>
+    <row r="96">
+      <c r="F96" s="11"/>
+      <c r="G96" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I96" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J96" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="K96" s="12"/>
+      <c r="L96" s="13"/>
+    </row>
+    <row r="97">
+      <c r="F97" s="11"/>
+      <c r="G97" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="J97" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="K97" s="12"/>
+      <c r="L97" s="13"/>
+    </row>
+    <row r="98">
+      <c r="F98" s="11"/>
+      <c r="G98" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="J98" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="K98" s="12"/>
+      <c r="L98" s="13"/>
+    </row>
+    <row r="99">
+      <c r="F99" s="11"/>
+      <c r="G99" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H99" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I99" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J99" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="K99" s="12"/>
+      <c r="L99" s="13"/>
+    </row>
+    <row r="100">
+      <c r="F100" s="11"/>
+      <c r="G100" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I100" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="J100" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="K100" s="12"/>
+      <c r="L100" s="13"/>
+    </row>
+    <row r="101">
+      <c r="F101" s="11"/>
+      <c r="G101" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H101" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I101" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="J101" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="K101" s="12"/>
+      <c r="L101" s="13"/>
+    </row>
+    <row r="102">
+      <c r="F102" s="11"/>
+      <c r="G102" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="J102" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="K102" s="12"/>
+      <c r="L102" s="13"/>
+    </row>
+    <row r="103">
+      <c r="F103" s="11"/>
+      <c r="G103" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H103" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I103" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="J103" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K103" s="12"/>
+      <c r="L103" s="13"/>
+    </row>
+    <row r="104">
+      <c r="F104" s="11"/>
+      <c r="G104" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="J104" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K104" s="12"/>
+      <c r="L104" s="13"/>
+    </row>
+    <row r="105">
+      <c r="F105" s="11"/>
+      <c r="G105" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H105" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I105" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="J105" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K105" s="12"/>
+      <c r="L105" s="13"/>
+    </row>
+    <row r="106">
+      <c r="F106" s="11"/>
+      <c r="G106" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H106" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I106" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="J106" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="K106" s="12"/>
+      <c r="L106" s="13"/>
+    </row>
+    <row r="107">
+      <c r="F107" s="11"/>
+      <c r="G107" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H107" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I107" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="J107" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="K107" s="12"/>
+      <c r="L107" s="13"/>
+    </row>
+    <row r="108">
+      <c r="F108" s="11"/>
+      <c r="G108" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H108" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="J108" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="K108" s="12"/>
+      <c r="L108" s="13"/>
+    </row>
+    <row r="109">
+      <c r="F109" s="11"/>
+      <c r="G109" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H109" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I109" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="J109" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="K109" s="15"/>
+      <c r="L109" s="16"/>
+    </row>
+    <row r="110">
+      <c r="F110" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="J110" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K110" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="L110" s="10"/>
+    </row>
+    <row r="111">
+      <c r="F111" s="11"/>
+      <c r="G111" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H111" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="J111" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="K111" s="12"/>
+      <c r="L111" s="13"/>
+    </row>
+    <row r="112">
+      <c r="F112" s="11"/>
+      <c r="G112" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="J112" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="K112" s="12"/>
+      <c r="L112" s="13"/>
+    </row>
+    <row r="113">
+      <c r="F113" s="11"/>
+      <c r="G113" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H113" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I113" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="J113" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K113" s="12"/>
+      <c r="L113" s="13"/>
+    </row>
+    <row r="114">
+      <c r="F114" s="11"/>
+      <c r="G114" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="J114" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K114" s="12"/>
+      <c r="L114" s="13"/>
+    </row>
+    <row r="115">
+      <c r="F115" s="11"/>
+      <c r="G115" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H115" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="J115" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K115" s="15"/>
+      <c r="L115" s="16"/>
+    </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="F69:F73"/>
-    <mergeCell ref="F74:F77"/>
-    <mergeCell ref="F78:F83"/>
+  <mergeCells count="22">
+    <mergeCell ref="K21:L30"/>
+    <mergeCell ref="K31:L42"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F14:F20"/>
+    <mergeCell ref="K14:L20"/>
     <mergeCell ref="F21:F30"/>
     <mergeCell ref="F31:F42"/>
-    <mergeCell ref="F43:F56"/>
-    <mergeCell ref="F57:F68"/>
-    <mergeCell ref="F14:F20"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K21:L30"/>
-    <mergeCell ref="K31:L42"/>
-    <mergeCell ref="K43:L56"/>
-    <mergeCell ref="K57:L68"/>
-    <mergeCell ref="K69:L73"/>
-    <mergeCell ref="K14:L20"/>
-    <mergeCell ref="K74:L77"/>
+    <mergeCell ref="K73:L77"/>
     <mergeCell ref="K78:L83"/>
+    <mergeCell ref="K61:L72"/>
+    <mergeCell ref="K84:L109"/>
+    <mergeCell ref="F110:F115"/>
+    <mergeCell ref="K110:L115"/>
+    <mergeCell ref="F43:F46"/>
+    <mergeCell ref="K43:L46"/>
+    <mergeCell ref="F47:F60"/>
+    <mergeCell ref="K47:L60"/>
+    <mergeCell ref="F61:F72"/>
+    <mergeCell ref="F73:F77"/>
+    <mergeCell ref="F84:F109"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>